<commit_message>
6/16/2024 - tambah module test game archived
</commit_message>
<xml_diff>
--- a/tugas tes case ppkpl.xlsx
+++ b/tugas tes case ppkpl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3841917163b10036/Documents/PPKPL/UAS_PPKPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEC8EF75-F4EB-4CC8-BC75-44BF1E7F63A1}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB37035-4741-481D-B997-FA2B16D8AB45}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t>App Name</t>
   </si>
@@ -215,19 +215,6 @@
   </si>
   <si>
     <t>Peringatan pengguna atau resource tidak ditemukan muncul</t>
-  </si>
-  <si>
-    <t>MG_004</t>
-  </si>
-  <si>
-    <t>Mengirim pesan tanpa isi pesan</t>
-  </si>
-  <si>
-    <t>1. Tekan tombol tab More
-2. Tekan tombol Message</t>
-  </si>
-  <si>
-    <t>Tombol kirim tidak ditampilkan</t>
   </si>
   <si>
     <t>Forum</t>
@@ -688,7 +675,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -700,33 +687,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -948,10 +908,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA215"/>
+  <dimension ref="A1:AA214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="63" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="63" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -975,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="5" t="s">
@@ -983,7 +943,7 @@
       </c>
       <c r="F1" s="22">
         <f ca="1">TODAY()</f>
-        <v>45458</v>
+        <v>45459</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -1004,7 +964,7 @@
       </c>
       <c r="F2" s="8">
         <f>COUNTIF(I:I,"PASSED")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1046,7 +1006,7 @@
       </c>
       <c r="F4" s="13">
         <f>SUM(F2:F3)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -1260,7 +1220,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>19</v>
@@ -1301,7 +1261,7 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>29</v>
@@ -1385,7 +1345,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>19</v>
@@ -1547,23 +1507,27 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="34.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="25"/>
+    <row r="17" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>3</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="C17" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>20</v>
@@ -1590,27 +1554,23 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <v>3</v>
-      </c>
-      <c r="B18" s="25" t="s">
+    <row r="18" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>87</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>49</v>
       </c>
       <c r="F18" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>72</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>20</v>
@@ -1637,23 +1597,23 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="25"/>
       <c r="C19" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>49</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>20</v>
@@ -1680,23 +1640,27 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="25"/>
+    <row r="20" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>4</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" s="19" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>20</v>
@@ -1723,27 +1687,23 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
-        <v>4</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>73</v>
-      </c>
+    <row r="21" spans="1:27" ht="139.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>75</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>20</v>
@@ -1770,23 +1730,23 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="139.19999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="25"/>
       <c r="C22" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>20</v>
@@ -1813,27 +1773,27 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="25"/>
+    <row r="23" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>5</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>84</v>
+      </c>
       <c r="C23" s="19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>49</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E23" s="19"/>
       <c r="F23" s="19" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="H23" s="19"/>
       <c r="I23" s="20" t="s">
         <v>21</v>
       </c>
@@ -1856,31 +1816,27 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
-        <v>5</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="19" t="s">
+    <row r="24" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="19"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="19"/>
+        <v>95</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="29"/>
       <c r="I24" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="29"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1903,17 +1859,17 @@
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>91</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H25" s="29"/>
       <c r="I25" s="20" t="s">
@@ -1938,27 +1894,15 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="29"/>
-      <c r="I26" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="29"/>
+    <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1982,6 +1926,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -7240,34 +7185,6 @@
       <c r="Z214" s="2"/>
       <c r="AA214" s="2"/>
     </row>
-    <row r="215" spans="2:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="2"/>
-      <c r="J215" s="2"/>
-      <c r="K215" s="2"/>
-      <c r="L215" s="2"/>
-      <c r="M215" s="2"/>
-      <c r="N215" s="2"/>
-      <c r="O215" s="2"/>
-      <c r="P215" s="2"/>
-      <c r="Q215" s="2"/>
-      <c r="R215" s="2"/>
-      <c r="S215" s="2"/>
-      <c r="T215" s="2"/>
-      <c r="U215" s="2"/>
-      <c r="V215" s="2"/>
-      <c r="W215" s="2"/>
-      <c r="X215" s="2"/>
-      <c r="Y215" s="2"/>
-      <c r="Z215" s="2"/>
-      <c r="AA215" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAILED">
@@ -7278,7 +7195,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="I10:I26" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I10:I25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PASSED,FAILED"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
tambah modul tes forum
</commit_message>
<xml_diff>
--- a/tugas tes case ppkpl.xlsx
+++ b/tugas tes case ppkpl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3841917163b10036/Documents/PPKPL/UAS_PPKPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB37035-4741-481D-B997-FA2B16D8AB45}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B6361A-10A3-40A3-8BE9-7CF5AFA472A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t>App Name</t>
   </si>
@@ -180,9 +180,6 @@
 5. Tekan simbol Kirim</t>
   </si>
   <si>
-    <t>Pesan diterima pengguna tujuan</t>
-  </si>
-  <si>
     <t>MG_002</t>
   </si>
   <si>
@@ -201,22 +198,6 @@
     <t>Peringatan tujuan pesan harus diisi muncul</t>
   </si>
   <si>
-    <t>MG_003</t>
-  </si>
-  <si>
-    <t>Mengirim pesan dengan tujuan pengguna tidak valid atau tidak ditemukan</t>
-  </si>
-  <si>
-    <t>1. Tekan tombol tab More
-2. Tekan tombol Message
-3. Input tujuan pesan dengan text random
-4. Input isi pesan
-5. Tekan simbol Kirim</t>
-  </si>
-  <si>
-    <t>Peringatan pengguna atau resource tidak ditemukan muncul</t>
-  </si>
-  <si>
     <t>Forum</t>
   </si>
   <si>
@@ -233,9 +214,6 @@
   </si>
   <si>
     <t>FM_003</t>
-  </si>
-  <si>
-    <t>Menambah komentar pada thread forum</t>
   </si>
   <si>
     <t>1. Tekan tombol tab More
@@ -252,23 +230,9 @@
 4. Tekan tombol create new topic</t>
   </si>
   <si>
-    <t>1. Tekan tombol tab More
-2. Tekan tombol forums
-3. Tekan satu thread forum
-4. Tekan tombol tulis komentar
-5. Input isi komentar
-6. Tekan tombol kirim</t>
-  </si>
-  <si>
-    <t>Komentar muncul di dalam thread forum</t>
-  </si>
-  <si>
     <t>Peringatan judul dan isi harus diisi muncul</t>
   </si>
   <si>
-    <t>Thread forum dengan judul, isi, dan nama pengguna yang sesuai dengan input muncul</t>
-  </si>
-  <si>
     <t>Game Archived</t>
   </si>
   <si>
@@ -281,12 +245,6 @@
     <t>User sudah login dan main satu game</t>
   </si>
   <si>
-    <t>1. Tekan tombol tab Mastery
-2. Tekan tombol Analysis
-3. Tekan tombol game archive
-4. Tekan game terbaru pada list game</t>
-  </si>
-  <si>
     <t>Game analysis activity di buka</t>
   </si>
   <si>
@@ -302,42 +260,15 @@
     <t>GA_003</t>
   </si>
   <si>
-    <t>1. Tekan tombol tab Mastery
-2. Tekan tombol Analysis
-3. Tekan tombol game archive
-4. Tekan tombol search
-5. Input tipe game Blitz
-6. Input I played as White
-7. Input result won
-8. Tekan tombol search</t>
-  </si>
-  <si>
-    <t>List game yang sesuai dengan filter muncul</t>
-  </si>
-  <si>
-    <t>1. Tekan tombol tab Mastery
-2. Tekan tombol Analysis
-3. Tekan tombol game archive
-4. Tekan tombol search
-5. Input filter tipe game yang tidak pernah dimainkan pengguna (Daily960, as black)
-8. Tekan tombol search</t>
-  </si>
-  <si>
     <t>Peringatan No results muncul pada list game</t>
   </si>
   <si>
-    <t>Posting thread baru di forum valid</t>
-  </si>
-  <si>
     <t>Lesson</t>
   </si>
   <si>
     <t>LS_001</t>
   </si>
   <si>
-    <t>Menampilkan lesson list sesuai dengan filter</t>
-  </si>
-  <si>
     <t>LS_002</t>
   </si>
   <si>
@@ -351,9 +282,6 @@
   </si>
   <si>
     <t>Lesson yang dicari tidak ditemukan</t>
-  </si>
-  <si>
-    <t>Memberikan list lesson yang sesuai dengan kata kunci pencarian</t>
   </si>
   <si>
     <t xml:space="preserve">Menampilkan text No Results </t>
@@ -399,6 +327,78 @@
 3. Input username "ozan.naufal16@gmail.com" 
 4. Input password yang benar
 5. Tekan tombol Log In</t>
+  </si>
+  <si>
+    <t>List game yang sesuai dengan filter muncul (game melawan user dengan nama "vasaa77")</t>
+  </si>
+  <si>
+    <t>1. Tekan tombol tab Mastery
+2. Tekan tombol Analysis
+3. Tekan tombol game archive
+4. Tekan tombol search
+5. Input tipe game Blitz
+6. Input result won
+7. Tekan tombol search</t>
+  </si>
+  <si>
+    <t>Menampilkan lesson list sesuai dengan filter (lesson dengan penulis "Thomas Wolsky" dan tingkat "Advanced")</t>
+  </si>
+  <si>
+    <t>Memberikan list lesson yang sesuai dengan kata kunci pencarian "Jeremy Silman"</t>
+  </si>
+  <si>
+    <t>1. Tekan tombol tab Mastery
+2. Tekan tombol Analysis
+3. Tekan tombol game archive
+4. Tekan tombol search
+5. Input filter tipe game yang tidak pernah dimainkan pengguna (hasil Draw)
+8. Tekan tombol search</t>
+  </si>
+  <si>
+    <t>1. Tekan tombol tab Mastery
+2. Tekan tombol Analysis
+3. Tekan tombol game archive
+4. Tekan game terbaru (paling atas) pada list game</t>
+  </si>
+  <si>
+    <t>Isi pesan muncul pada list pesan</t>
+  </si>
+  <si>
+    <t>Search topic di forum</t>
+  </si>
+  <si>
+    <t>1. Tekan tombol tab More
+2. Tekan tombol forums
+3. Tekan simbol search
+4. Input kata kunci "Do you Believe in Religion"
+5. ganti kategori menjadi "All"
+6. Tekan tombol search</t>
+  </si>
+  <si>
+    <t>Topic dengan judul "Do you Believe in Religion" muncul pada list topic forum</t>
+  </si>
+  <si>
+    <t>peringatan untuk login terlebih dahulu muncul</t>
+  </si>
+  <si>
+    <t>1. Tekan tombol tab More
+2. Tekan tombol forums
+3. Tekan simbol search
+4. Input kata kunci "129321333103984"
+5. ganti kategori menjadi "All"
+6. Tekan tombol search</t>
+  </si>
+  <si>
+    <t>Search topic di forum hasil tidak ditemukan</t>
+  </si>
+  <si>
+    <t>FM_004</t>
+  </si>
+  <si>
+    <t>Text "No Forum Topics" muncul pada list topic forum</t>
+  </si>
+  <si>
+    <t>Posting topic baru di forum tidak login</t>
   </si>
 </sst>
 </file>
@@ -910,8 +910,8 @@
   </sheetPr>
   <dimension ref="A1:AA214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="63" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="5" t="s">
@@ -1220,7 +1220,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>19</v>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>29</v>
@@ -1345,7 +1345,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>19</v>
@@ -1389,13 +1389,13 @@
         <v>44</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>45</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>20</v>
@@ -1425,19 +1425,19 @@
     <row r="15" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
       <c r="C15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="G15" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>20</v>
@@ -1464,23 +1464,25 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="87" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="25"/>
+    <row r="16" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>3</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="C16" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>49</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E16" s="19"/>
       <c r="F16" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>20</v>
@@ -1508,26 +1510,20 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>3</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>56</v>
-      </c>
+      <c r="A17" s="21"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>49</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E17" s="19"/>
       <c r="F17" s="19" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>20</v>
@@ -1554,23 +1550,21 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="25"/>
       <c r="C18" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>49</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E18" s="19"/>
       <c r="F18" s="19" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>20</v>
@@ -1597,23 +1591,21 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="25"/>
       <c r="C19" s="19" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>49</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E19" s="19"/>
       <c r="F19" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>20</v>
@@ -1645,22 +1637,22 @@
         <v>4</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>20</v>
@@ -1687,23 +1679,23 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="139.19999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="25"/>
       <c r="C21" s="19" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>20</v>
@@ -1734,19 +1726,19 @@
       <c r="A22" s="21"/>
       <c r="B22" s="25"/>
       <c r="C22" s="19" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>20</v>
@@ -1778,22 +1770,24 @@
         <v>5</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="I23" s="20" t="s">
         <v>21</v>
       </c>
@@ -1820,19 +1814,21 @@
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="19" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="I24" s="20" t="s">
         <v>21</v>
       </c>
@@ -1859,19 +1855,21 @@
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="19" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="29"/>
+        <v>77</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="I25" s="20" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
6/16/2024 - tambah modul tes forum
</commit_message>
<xml_diff>
--- a/tugas tes case ppkpl.xlsx
+++ b/tugas tes case ppkpl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3841917163b10036/Documents/PPKPL/UAS_PPKPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B6361A-10A3-40A3-8BE9-7CF5AFA472A6}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{1B5DF3B9-1803-4AFA-8F84-C67AF5CB609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87EE95E6-094A-42A3-BE15-F48146133EB2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
   <si>
     <t>App Name</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>FM_002</t>
-  </si>
-  <si>
-    <t>Posting di forum tanpa judul dan isi</t>
   </si>
   <si>
     <t>FM_003</t>
@@ -222,15 +219,6 @@
 4. Input judul thread
 5. Input isi thread
 6. Tekan tombol create new topic</t>
-  </si>
-  <si>
-    <t>1. Tekan tombol tab More
-2. Tekan tombol forums
-3. Tekan simbol tambah
-4. Tekan tombol create new topic</t>
-  </si>
-  <si>
-    <t>Peringatan judul dan isi harus diisi muncul</t>
   </si>
   <si>
     <t>Game Archived</t>
@@ -390,9 +378,6 @@
   </si>
   <si>
     <t>Search topic di forum hasil tidak ditemukan</t>
-  </si>
-  <si>
-    <t>FM_004</t>
   </si>
   <si>
     <t>Text "No Forum Topics" muncul pada list topic forum</t>
@@ -908,10 +893,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA214"/>
+  <dimension ref="A1:AA213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -942,7 +927,6 @@
         <v>1</v>
       </c>
       <c r="F1" s="22">
-        <f ca="1">TODAY()</f>
         <v>45459</v>
       </c>
       <c r="G1" s="4"/>
@@ -964,7 +948,7 @@
       </c>
       <c r="F2" s="8">
         <f>COUNTIF(I:I,"PASSED")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1006,7 +990,7 @@
       </c>
       <c r="F4" s="13">
         <f>SUM(F2:F3)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -1220,7 +1204,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>19</v>
@@ -1261,7 +1245,7 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>29</v>
@@ -1345,7 +1329,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>19</v>
@@ -1395,7 +1379,7 @@
         <v>45</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>20</v>
@@ -1475,14 +1459,14 @@
         <v>52</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>20</v>
@@ -1516,14 +1500,14 @@
         <v>54</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>20</v>
@@ -1554,17 +1538,17 @@
       <c r="A18" s="21"/>
       <c r="B18" s="25"/>
       <c r="C18" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>20</v>
@@ -1592,20 +1576,26 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="21">
+        <v>4</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" s="19" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="F19" s="19" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>20</v>
@@ -1632,27 +1622,23 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
-        <v>4</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>60</v>
-      </c>
+    <row r="20" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>20</v>
@@ -1679,23 +1665,23 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="25"/>
       <c r="C21" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>85</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>20</v>
@@ -1722,23 +1708,25 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="104.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="25"/>
+    <row r="22" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>5</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="C22" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>48</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E22" s="19"/>
       <c r="F22" s="19" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>20</v>
@@ -1765,25 +1753,21 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="121.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
-        <v>5</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="19" t="s">
+    <row r="23" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>20</v>
@@ -1791,7 +1775,7 @@
       <c r="I23" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1814,17 +1798,17 @@
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>20</v>
@@ -1851,29 +1835,15 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="29"/>
+    <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1897,6 +1867,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -7155,34 +7126,6 @@
       <c r="Z213" s="2"/>
       <c r="AA213" s="2"/>
     </row>
-    <row r="214" spans="2:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
-      <c r="D214" s="2"/>
-      <c r="E214" s="2"/>
-      <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-      <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
-      <c r="L214" s="2"/>
-      <c r="M214" s="2"/>
-      <c r="N214" s="2"/>
-      <c r="O214" s="2"/>
-      <c r="P214" s="2"/>
-      <c r="Q214" s="2"/>
-      <c r="R214" s="2"/>
-      <c r="S214" s="2"/>
-      <c r="T214" s="2"/>
-      <c r="U214" s="2"/>
-      <c r="V214" s="2"/>
-      <c r="W214" s="2"/>
-      <c r="X214" s="2"/>
-      <c r="Y214" s="2"/>
-      <c r="Z214" s="2"/>
-      <c r="AA214" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAILED">
@@ -7193,7 +7136,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="I10:I25" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I10:I24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PASSED,FAILED"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>